<commit_message>
Tidy SDOH tab; Add mean age sorting options
</commit_message>
<xml_diff>
--- a/myCCB/Standards/ageLink.xlsx
+++ b/myCCB/Standards/ageLink.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693D2FC9-4A71-4DDB-AF44-A349DF19EE96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1FDE15-EF65-4ED6-A8A0-8BF5D2A325D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age3" sheetId="5" r:id="rId1"/>
@@ -288,13 +288,13 @@
     <t>95 - 99</t>
   </si>
   <si>
-    <t>100 - 199</t>
-  </si>
-  <si>
     <t>t</t>
   </si>
   <si>
     <t>u</t>
+  </si>
+  <si>
+    <t>100+</t>
   </si>
 </sst>
 </file>
@@ -2079,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7366E3D-F6DF-433C-8A0F-34DEB12ACD6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,7 +2348,7 @@
         <v>199</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>58</v>
@@ -2363,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F9D75C-EBDD-4A61-A882-10D4334AEA9F}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2660,7 +2660,7 @@
         <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2671,10 +2671,10 @@
         <v>199</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CCB Jan 1 push: condition list updates & 2021 HCAI data
</commit_message>
<xml_diff>
--- a/myCCB/Standards/ageLink.xlsx
+++ b/myCCB/Standards/ageLink.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1FDE15-EF65-4ED6-A8A0-8BF5D2A325D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564BE5DC-A28B-46A7-85FA-B64897F96BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age3" sheetId="5" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="standard" sheetId="9" r:id="rId11"/>
     <sheet name="multi" sheetId="6" r:id="rId12"/>
     <sheet name="ageLE" sheetId="11" r:id="rId13"/>
+    <sheet name="ageLE_mssa" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="86">
   <si>
     <t>ageName</t>
   </si>
@@ -1116,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624E9647-ABC4-418E-873B-6006FDFAB2E5}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,6 +1409,230 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043D821A-0B90-4949-B080-DD1FAD7B887D}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>49</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>54</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>59</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>64</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>69</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>74</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <v>79</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>84</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <v>199</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2079,7 +2304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7366E3D-F6DF-433C-8A0F-34DEB12ACD6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Clean up IHME files; Life tables work
</commit_message>
<xml_diff>
--- a/myCCB/Standards/ageLink.xlsx
+++ b/myCCB/Standards/ageLink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D03496-4D85-40B7-BBB9-77A862BC08B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB855C65-70E5-424F-A112-5581E16FB6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="13155" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age3" sheetId="5" r:id="rId1"/>
@@ -20,14 +20,14 @@
     <sheet name="age6" sheetId="3" r:id="rId5"/>
     <sheet name="age7" sheetId="10" r:id="rId6"/>
     <sheet name="age8" sheetId="1" r:id="rId7"/>
-    <sheet name="age11" sheetId="15" r:id="rId8"/>
-    <sheet name="age18" sheetId="12" r:id="rId9"/>
-    <sheet name="age21" sheetId="13" r:id="rId10"/>
-    <sheet name="ageAdult" sheetId="8" r:id="rId11"/>
-    <sheet name="standard" sheetId="9" r:id="rId12"/>
-    <sheet name="multi" sheetId="6" r:id="rId13"/>
-    <sheet name="ageLE" sheetId="11" r:id="rId14"/>
-    <sheet name="ageLE_mssa" sheetId="14" r:id="rId15"/>
+    <sheet name="age18" sheetId="12" r:id="rId8"/>
+    <sheet name="age21" sheetId="13" r:id="rId9"/>
+    <sheet name="ageAdult" sheetId="8" r:id="rId10"/>
+    <sheet name="standard" sheetId="9" r:id="rId11"/>
+    <sheet name="multi" sheetId="6" r:id="rId12"/>
+    <sheet name="ageLE" sheetId="11" r:id="rId13"/>
+    <sheet name="ageLE_mssa" sheetId="14" r:id="rId14"/>
+    <sheet name="ageLE_tract" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -740,330 +740,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F9D75C-EBDD-4A61-A882-10D4334AEA9F}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>29</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <v>34</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <v>39</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>40</v>
-      </c>
-      <c r="B10">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>45</v>
-      </c>
-      <c r="B11">
-        <v>49</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <v>54</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>55</v>
-      </c>
-      <c r="B13">
-        <v>59</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>60</v>
-      </c>
-      <c r="B14">
-        <v>64</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>65</v>
-      </c>
-      <c r="B15">
-        <v>69</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>70</v>
-      </c>
-      <c r="B16">
-        <v>74</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>75</v>
-      </c>
-      <c r="B17">
-        <v>79</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>80</v>
-      </c>
-      <c r="B18">
-        <v>84</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>85</v>
-      </c>
-      <c r="B19">
-        <v>89</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>90</v>
-      </c>
-      <c r="B20">
-        <v>94</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>95</v>
-      </c>
-      <c r="B21">
-        <v>99</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>100</v>
-      </c>
-      <c r="B22">
-        <v>199</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1120,7 +796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -1290,7 +966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:G10"/>
   <sheetViews>
@@ -1444,11 +1120,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624E9647-ABC4-418E-873B-6006FDFAB2E5}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -1743,12 +1419,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043D821A-0B90-4949-B080-DD1FAD7B887D}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,6 +1636,189 @@
       </c>
       <c r="C19" s="4" t="s">
         <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A1E180-7C20-4821-ACDE-9D08839FA4F5}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>54</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>64</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>74</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <v>84</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>85</v>
+      </c>
+      <c r="B12">
+        <v>199</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2632,189 +2491,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A1E180-7C20-4821-ACDE-9D08839FA4F5}">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>24</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>34</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>35</v>
-      </c>
-      <c r="B7">
-        <v>44</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>45</v>
-      </c>
-      <c r="B8">
-        <v>54</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>55</v>
-      </c>
-      <c r="B9">
-        <v>64</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>65</v>
-      </c>
-      <c r="B10">
-        <v>74</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>75</v>
-      </c>
-      <c r="B11">
-        <v>84</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>85</v>
-      </c>
-      <c r="B12">
-        <v>199</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7366E3D-F6DF-433C-8A0F-34DEB12ACD6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -3096,4 +2772,328 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F9D75C-EBDD-4A61-A882-10D4334AEA9F}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>49</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>54</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>59</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>64</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>69</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>74</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <v>79</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>84</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <v>89</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>90</v>
+      </c>
+      <c r="B20">
+        <v>94</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>95</v>
+      </c>
+      <c r="B21">
+        <v>99</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <v>199</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>